<commit_message>
Wheels, tools, retracting wire
Corrected errors. Added 2 standard wheels, two sets of standard
allen-Keys, one chain breaker, and a 2ft section of retractable wire (18
ga).
</commit_message>
<xml_diff>
--- a/Phi Alpha/Hardware Master Equipment List/Master_Equipment_List_PhiAlpha452.xlsx
+++ b/Phi Alpha/Hardware Master Equipment List/Master_Equipment_List_PhiAlpha452.xlsx
@@ -7,9 +7,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="order" sheetId="2" r:id="rId1"/>
-    <sheet name="order (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="order (3)" sheetId="4" r:id="rId1"/>
+    <sheet name="order" sheetId="2" r:id="rId2"/>
+    <sheet name="order (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -56,7 +57,7 @@
     <author>Mike McMillan</author>
   </authors>
   <commentList>
-    <comment ref="I34" authorId="0">
+    <comment ref="J56" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,8 +121,43 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Mike McMillan</author>
+  </authors>
+  <commentList>
+    <comment ref="I34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mike McMillan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+MAY NOT NEED FOR NEW ELECTIONICS
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="259">
   <si>
     <t>part Number</t>
   </si>
@@ -853,6 +889,51 @@
   </si>
   <si>
     <t>Gears</t>
+  </si>
+  <si>
+    <t>Wires</t>
+  </si>
+  <si>
+    <t>Coiled wire (McMaster-Carr)</t>
+  </si>
+  <si>
+    <t>Power (14 gauge (black white)</t>
+  </si>
+  <si>
+    <t>thread pulleys</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (McMaster-Carr)</t>
+  </si>
+  <si>
+    <t>Retracting Cable (300V AC-Light Duty)</t>
+  </si>
+  <si>
+    <t>18 Gauge 2 wire</t>
+  </si>
+  <si>
+    <t>TETRIX MAX Omni Wheel Pack</t>
+  </si>
+  <si>
+    <t>4 inch</t>
+  </si>
+  <si>
+    <t>W36466</t>
+  </si>
+  <si>
+    <t>W39104</t>
+  </si>
+  <si>
+    <t>7/64, 3/32, 1/16, 5/64</t>
+  </si>
+  <si>
+    <t>7088k211</t>
+  </si>
+  <si>
+    <t>2ft, 18ga</t>
+  </si>
+  <si>
+    <t>4"</t>
   </si>
 </sst>
 </file>
@@ -1235,12 +1316,2035 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="660" topLeftCell="A16" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="795" topLeftCell="A62" activePane="bottomLeft"/>
+      <selection activeCell="D13" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="6" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="4"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4">
+        <v>17.95</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4">
+        <f>H3*J3</f>
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="4">
+        <v>27.95</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <f>H4*J4</f>
+        <v>27.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="4">
+        <v>16.95</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <f>H5*J5</f>
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="B6" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="4">
+        <v>11.95</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3</v>
+      </c>
+      <c r="K6" s="4">
+        <f>H6*J6</f>
+        <v>35.849999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2</v>
+      </c>
+      <c r="J7" s="5">
+        <v>2</v>
+      </c>
+      <c r="K7" s="4">
+        <f>H7*J7</f>
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="B10" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="4">
+        <v>5.95</v>
+      </c>
+      <c r="I10" s="5">
+        <v>2</v>
+      </c>
+      <c r="J10" s="5">
+        <v>4</v>
+      </c>
+      <c r="K10" s="4">
+        <f>H10*J10</f>
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" hidden="1">
+      <c r="B11" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="I11" s="5">
+        <v>2</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <f>H11*J11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="I12" s="5">
+        <v>2</v>
+      </c>
+      <c r="J12" s="5">
+        <v>3</v>
+      </c>
+      <c r="K12" s="4">
+        <f>H12*J12</f>
+        <v>14.850000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="B13" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="I13" s="5">
+        <v>2</v>
+      </c>
+      <c r="J13" s="5">
+        <v>4</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" ref="K13" si="0">H13*J13</f>
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="B16" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="4">
+        <v>13.95</v>
+      </c>
+      <c r="I16" s="5">
+        <v>2</v>
+      </c>
+      <c r="J16" s="5">
+        <v>2</v>
+      </c>
+      <c r="K16" s="4">
+        <f>H16*J16</f>
+        <v>27.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="B17" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="4">
+        <v>10.95</v>
+      </c>
+      <c r="I17" s="5">
+        <v>2</v>
+      </c>
+      <c r="J17" s="5">
+        <v>2</v>
+      </c>
+      <c r="K17" s="4">
+        <f>H17*J17</f>
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="B20" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="4">
+        <v>12.95</v>
+      </c>
+      <c r="I20" s="5">
+        <v>2</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4">
+        <f>H20*J20</f>
+        <v>12.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="B23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="4">
+        <v>15.95</v>
+      </c>
+      <c r="I23" s="5">
+        <v>6</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1</v>
+      </c>
+      <c r="K23" s="4">
+        <f>H23*J23</f>
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="B24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="4">
+        <v>15.95</v>
+      </c>
+      <c r="I24" s="5">
+        <v>3</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1</v>
+      </c>
+      <c r="K24" s="4">
+        <f>H24*J24</f>
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" hidden="1">
+      <c r="B25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="4">
+        <v>6.95</v>
+      </c>
+      <c r="I25" s="5">
+        <v>2</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4">
+        <f>H25*J25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" customFormat="1">
+      <c r="A26" s="5"/>
+      <c r="B26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" ref="K26" si="1">H26*J26</f>
+        <v>27.8</v>
+      </c>
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="B27" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="4">
+        <v>3.95</v>
+      </c>
+      <c r="I27" s="5">
+        <v>6</v>
+      </c>
+      <c r="J27" s="5">
+        <v>2</v>
+      </c>
+      <c r="K27" s="4">
+        <f>H27*J27</f>
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" hidden="1">
+      <c r="B28" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="I28" s="5">
+        <v>12</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
+        <f>H28*J28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" hidden="1">
+      <c r="B29" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="I29" s="5">
+        <v>6</v>
+      </c>
+      <c r="J29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <f>H29*J29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="B32" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="4">
+        <v>13.95</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" s="5">
+        <v>1</v>
+      </c>
+      <c r="K32" s="4">
+        <f>H32*J32</f>
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="B33" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E33" s="5">
+        <v>32</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="4">
+        <v>29.95</v>
+      </c>
+      <c r="I33" s="5">
+        <v>2</v>
+      </c>
+      <c r="J33" s="5">
+        <v>1</v>
+      </c>
+      <c r="K33" s="4">
+        <f t="shared" ref="K33:K35" si="2">H33*J33</f>
+        <v>29.95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="B34" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E34" s="5">
+        <v>24</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="4">
+        <v>22.95</v>
+      </c>
+      <c r="I34" s="5">
+        <v>2</v>
+      </c>
+      <c r="J34" s="5">
+        <v>2</v>
+      </c>
+      <c r="K34" s="4">
+        <f t="shared" si="2"/>
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="B35" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E35" s="5">
+        <v>16</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="4">
+        <v>16.95</v>
+      </c>
+      <c r="I35" s="5">
+        <v>2</v>
+      </c>
+      <c r="J35" s="5">
+        <v>2</v>
+      </c>
+      <c r="K35" s="4">
+        <f t="shared" si="2"/>
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="B38" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="4">
+        <v>27.95</v>
+      </c>
+      <c r="I38" s="5">
+        <v>2</v>
+      </c>
+      <c r="J38" s="5">
+        <v>1</v>
+      </c>
+      <c r="K38" s="4">
+        <f t="shared" ref="K38:K43" si="3">H38*J38</f>
+        <v>27.95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" hidden="1">
+      <c r="B39" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="4">
+        <v>17.95</v>
+      </c>
+      <c r="I39" s="5">
+        <v>1</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0</v>
+      </c>
+      <c r="K39" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" hidden="1">
+      <c r="B40" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="4">
+        <v>22.95</v>
+      </c>
+      <c r="I40" s="5">
+        <v>2</v>
+      </c>
+      <c r="J40" s="5">
+        <v>0</v>
+      </c>
+      <c r="K40" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="B41" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="4">
+        <v>6.95</v>
+      </c>
+      <c r="I41" s="5">
+        <v>2</v>
+      </c>
+      <c r="J41" s="5">
+        <v>4</v>
+      </c>
+      <c r="K41" s="4">
+        <f t="shared" si="3"/>
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" hidden="1">
+      <c r="B42" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="4">
+        <v>29.95</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" hidden="1">
+      <c r="B43" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="4">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0</v>
+      </c>
+      <c r="K43" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" hidden="1">
+      <c r="B46" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H46" s="4">
+        <v>25</v>
+      </c>
+      <c r="I46" s="5">
+        <v>1</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4">
+        <f t="shared" ref="K46:K56" si="4">H46*J46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" hidden="1">
+      <c r="B47" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="4">
+        <v>24.95</v>
+      </c>
+      <c r="I47" s="5">
+        <v>1</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" hidden="1">
+      <c r="B48" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="4">
+        <v>5.95</v>
+      </c>
+      <c r="I48" s="5">
+        <v>2</v>
+      </c>
+      <c r="J48" s="5">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" hidden="1">
+      <c r="B49" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" s="4">
+        <v>15.95</v>
+      </c>
+      <c r="I49" s="5">
+        <v>1</v>
+      </c>
+      <c r="J49" s="5">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="12" hidden="1" customHeight="1">
+      <c r="B50" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H50" s="4">
+        <v>15.95</v>
+      </c>
+      <c r="I50" s="5">
+        <v>1</v>
+      </c>
+      <c r="J50" s="5">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M50" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" hidden="1">
+      <c r="B51" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="4">
+        <v>15.95</v>
+      </c>
+      <c r="I51" s="5">
+        <v>1</v>
+      </c>
+      <c r="J51" s="5">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" hidden="1">
+      <c r="C52" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J52" s="5">
+        <v>0</v>
+      </c>
+      <c r="K52" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="B53" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="I53" s="5">
+        <v>1</v>
+      </c>
+      <c r="J53" s="5">
+        <v>2</v>
+      </c>
+      <c r="K53" s="4">
+        <f t="shared" si="4"/>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" hidden="1">
+      <c r="B54" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="I54" s="5">
+        <v>1</v>
+      </c>
+      <c r="J54" s="5">
+        <v>0</v>
+      </c>
+      <c r="K54" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="25.5">
+      <c r="B55" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H55" s="4">
+        <v>5</v>
+      </c>
+      <c r="I55" s="5">
+        <v>1</v>
+      </c>
+      <c r="J55" s="5">
+        <v>4</v>
+      </c>
+      <c r="K55" s="4">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" hidden="1">
+      <c r="B56" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="4">
+        <v>79.95</v>
+      </c>
+      <c r="I56" s="5">
+        <v>1</v>
+      </c>
+      <c r="J56" s="5">
+        <v>0</v>
+      </c>
+      <c r="K56" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="16.5" customHeight="1">
+      <c r="A58" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" hidden="1">
+      <c r="B59" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="4">
+        <v>24.95</v>
+      </c>
+      <c r="I59" s="5">
+        <v>1</v>
+      </c>
+      <c r="J59" s="5">
+        <v>0</v>
+      </c>
+      <c r="K59" s="4">
+        <f>H59*J59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="25.5">
+      <c r="B60" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I60" s="5">
+        <v>2</v>
+      </c>
+      <c r="J60" s="5">
+        <v>1</v>
+      </c>
+      <c r="K60" s="4">
+        <f>H60*J60</f>
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="25.5" hidden="1">
+      <c r="B61" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="4">
+        <v>24.95</v>
+      </c>
+      <c r="I61" s="5">
+        <v>1</v>
+      </c>
+      <c r="J61" s="5">
+        <v>0</v>
+      </c>
+      <c r="K61" s="4">
+        <f t="shared" ref="K61" si="5">H61*J61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="14.25" customHeight="1">
+      <c r="A63" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" hidden="1">
+      <c r="B64" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="4">
+        <v>89.95</v>
+      </c>
+      <c r="I64" s="5">
+        <v>1</v>
+      </c>
+      <c r="J64" s="5">
+        <v>0</v>
+      </c>
+      <c r="K64" s="4">
+        <f>H64*J64</f>
+        <v>0</v>
+      </c>
+      <c r="M64" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" hidden="1">
+      <c r="C65" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J65" s="5">
+        <v>0</v>
+      </c>
+      <c r="K65" s="4">
+        <f>H65*J65</f>
+        <v>0</v>
+      </c>
+      <c r="M65" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" hidden="1">
+      <c r="B66" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H66" s="4">
+        <v>79.95</v>
+      </c>
+      <c r="I66" s="5">
+        <v>1</v>
+      </c>
+      <c r="J66" s="5">
+        <v>0</v>
+      </c>
+      <c r="K66" s="4">
+        <f>H66*J66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="68" spans="1:13" ht="17.25" customHeight="1">
+      <c r="A68" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="14.25" hidden="1" customHeight="1">
+      <c r="C69" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="16.5" customHeight="1">
+      <c r="B70" t="s">
+        <v>256</v>
+      </c>
+      <c r="C70" t="s">
+        <v>249</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E70" t="s">
+        <v>257</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="H70" s="4">
+        <v>25.52</v>
+      </c>
+      <c r="I70" s="5">
+        <v>1</v>
+      </c>
+      <c r="J70" s="5">
+        <v>1</v>
+      </c>
+      <c r="K70" s="4">
+        <f>H70*J70</f>
+        <v>25.52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="16.5" customHeight="1">
+      <c r="C71"/>
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:13" ht="14.25" customHeight="1">
+      <c r="A72" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C72"/>
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:13" ht="12.75" customHeight="1">
+      <c r="B73" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H73" s="4">
+        <v>19.95</v>
+      </c>
+      <c r="I73" s="5">
+        <v>1</v>
+      </c>
+      <c r="J73" s="5">
+        <v>2</v>
+      </c>
+      <c r="K73" s="4">
+        <f>H73*J73</f>
+        <v>39.9</v>
+      </c>
+      <c r="M73" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="16.5" hidden="1" customHeight="1">
+      <c r="B74" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H74" s="4">
+        <v>29.95</v>
+      </c>
+      <c r="I74" s="5">
+        <v>2</v>
+      </c>
+      <c r="J74" s="5">
+        <v>0</v>
+      </c>
+      <c r="K74" s="4">
+        <f>H74*J74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="16.5" customHeight="1">
+      <c r="B75" t="s">
+        <v>253</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E75" t="s">
+        <v>258</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H75" s="4">
+        <v>29.95</v>
+      </c>
+      <c r="I75" s="5">
+        <v>2</v>
+      </c>
+      <c r="J75" s="5">
+        <v>1</v>
+      </c>
+      <c r="K75" s="4">
+        <v>29.95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" hidden="1">
+      <c r="B78" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I78" s="5">
+        <v>100</v>
+      </c>
+      <c r="J78" s="5">
+        <v>0</v>
+      </c>
+      <c r="K78" s="4">
+        <f t="shared" ref="K78:K94" si="6">H78*J78</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" hidden="1">
+      <c r="B79" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H79" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I79" s="5">
+        <v>100</v>
+      </c>
+      <c r="J79" s="5">
+        <v>0</v>
+      </c>
+      <c r="K79" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" hidden="1">
+      <c r="B80" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H80" s="4">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I80" s="5">
+        <v>50</v>
+      </c>
+      <c r="J80" s="5">
+        <v>0</v>
+      </c>
+      <c r="K80" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" hidden="1">
+      <c r="B81" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H81" s="4">
+        <v>2.95</v>
+      </c>
+      <c r="I81" s="5">
+        <v>100</v>
+      </c>
+      <c r="J81" s="5">
+        <v>0</v>
+      </c>
+      <c r="K81" s="4">
+        <f>H81*J81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" hidden="1">
+      <c r="B82" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H82" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I82" s="5">
+        <v>100</v>
+      </c>
+      <c r="J82" s="5">
+        <v>0</v>
+      </c>
+      <c r="K82" s="4">
+        <f>H82*J82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="17.25" hidden="1" customHeight="1">
+      <c r="B83" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H83" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I83" s="5">
+        <v>100</v>
+      </c>
+      <c r="J83" s="5">
+        <v>0</v>
+      </c>
+      <c r="K83" s="4">
+        <f>H83*J83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" hidden="1">
+      <c r="B84" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H84" s="4">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I84" s="5">
+        <v>50</v>
+      </c>
+      <c r="J84" s="5">
+        <v>0</v>
+      </c>
+      <c r="K84" s="4">
+        <f>H84*J84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" hidden="1">
+      <c r="B88" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H88" s="4">
+        <v>49.95</v>
+      </c>
+      <c r="I88" s="5">
+        <v>1</v>
+      </c>
+      <c r="J88" s="5">
+        <v>0</v>
+      </c>
+      <c r="K88" s="4">
+        <f>H88*J88</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" hidden="1">
+      <c r="B89" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H89" s="4">
+        <v>5.95</v>
+      </c>
+      <c r="I89" s="5">
+        <v>1</v>
+      </c>
+      <c r="J89" s="5">
+        <v>0</v>
+      </c>
+      <c r="K89" s="4">
+        <f>H89*J89</f>
+        <v>0</v>
+      </c>
+      <c r="L89" s="11"/>
+    </row>
+    <row r="90" spans="1:12" hidden="1">
+      <c r="B90" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H90" s="4">
+        <v>24.95</v>
+      </c>
+      <c r="I90" s="5">
+        <v>1</v>
+      </c>
+      <c r="J90" s="5">
+        <v>0</v>
+      </c>
+      <c r="K90" s="4">
+        <f>H90*J90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="B93" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H93" s="4">
+        <v>16.95</v>
+      </c>
+      <c r="J93" s="5">
+        <v>1</v>
+      </c>
+      <c r="K93" s="4">
+        <f t="shared" si="6"/>
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="B94" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E94" t="s">
+        <v>255</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H94" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="I94" t="s">
+        <v>50</v>
+      </c>
+      <c r="J94" s="5">
+        <v>2</v>
+      </c>
+      <c r="K94" s="4">
+        <f t="shared" si="6"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" hidden="1">
+      <c r="B97" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E97" s="5">
+        <v>346</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H97" s="4">
+        <v>27.17</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J97" s="5">
+        <v>0</v>
+      </c>
+      <c r="K97" s="4">
+        <f>H97*J97</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" hidden="1">
+      <c r="B98" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E98" s="5">
+        <v>693</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H98" s="4">
+        <v>12.77</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J98" s="5">
+        <v>0</v>
+      </c>
+      <c r="K98" s="4">
+        <f>H98*J98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" hidden="1">
+      <c r="B99" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H99" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="I99" s="5">
+        <v>1</v>
+      </c>
+      <c r="J99" s="5">
+        <v>0</v>
+      </c>
+      <c r="K99" s="4">
+        <f>H99*J99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11">
+      <c r="B102" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H102" s="4">
+        <v>3.95</v>
+      </c>
+      <c r="I102" s="5">
+        <v>12</v>
+      </c>
+      <c r="J102" s="5">
+        <v>1</v>
+      </c>
+      <c r="K102" s="4">
+        <f>H102*J102</f>
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11">
+      <c r="B103" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H103" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="I103" s="5">
+        <v>12</v>
+      </c>
+      <c r="J103" s="5">
+        <v>1</v>
+      </c>
+      <c r="K103" s="4">
+        <f>H103*J103</f>
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11" hidden="1">
+      <c r="B104" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H104" s="4">
+        <v>13.95</v>
+      </c>
+      <c r="I104" s="5">
+        <v>12</v>
+      </c>
+      <c r="J104" s="5">
+        <v>0</v>
+      </c>
+      <c r="K104" s="4">
+        <f>H104*J104</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:11" hidden="1">
+      <c r="B105" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H105" s="4">
+        <v>12</v>
+      </c>
+      <c r="I105" s="5">
+        <v>12</v>
+      </c>
+      <c r="J105" s="5">
+        <v>0</v>
+      </c>
+      <c r="K105" s="4">
+        <f>H105*J105</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:11">
+      <c r="K108" s="4">
+        <f>SUM(K2:K107)</f>
+        <v>661.77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M106"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="660" topLeftCell="A50" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1975,7 +4079,7 @@
         <v>1</v>
       </c>
       <c r="K38" s="4">
-        <f>H38*J38</f>
+        <f t="shared" ref="K38:K43" si="3">H38*J38</f>
         <v>27.95</v>
       </c>
     </row>
@@ -2002,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="4">
-        <f>H39*J39</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2029,7 +4133,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="4">
-        <f>H40*J40</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2056,7 +4160,7 @@
         <v>4</v>
       </c>
       <c r="K41" s="4">
-        <f>H41*J41</f>
+        <f t="shared" si="3"/>
         <v>27.8</v>
       </c>
     </row>
@@ -2080,7 +4184,7 @@
         <v>1</v>
       </c>
       <c r="K42" s="4">
-        <f>H42*J42</f>
+        <f t="shared" si="3"/>
         <v>29.95</v>
       </c>
     </row>
@@ -2107,7 +4211,7 @@
         <v>1</v>
       </c>
       <c r="K43" s="4">
-        <f>H43*J43</f>
+        <f t="shared" si="3"/>
         <v>34.950000000000003</v>
       </c>
     </row>
@@ -2142,7 +4246,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="4">
-        <f>H46*J46</f>
+        <f t="shared" ref="K46:K56" si="4">H46*J46</f>
         <v>0</v>
       </c>
     </row>
@@ -2169,7 +4273,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="4">
-        <f>H47*J47</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L47" s="5" t="s">
@@ -2202,7 +4306,7 @@
         <v>1</v>
       </c>
       <c r="K48" s="4">
-        <f>H48*J48</f>
+        <f t="shared" si="4"/>
         <v>5.95</v>
       </c>
     </row>
@@ -2226,7 +4330,7 @@
         <v>0</v>
       </c>
       <c r="K49" s="4">
-        <f>H49*J49</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2253,7 +4357,7 @@
         <v>4</v>
       </c>
       <c r="K50" s="4">
-        <f>H50*J50</f>
+        <f t="shared" si="4"/>
         <v>63.8</v>
       </c>
       <c r="M50" s="5" t="s">
@@ -2283,7 +4387,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="4">
-        <f>H51*J51</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2301,7 +4405,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="4">
-        <f>H52*J52</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2325,7 +4429,7 @@
         <v>6</v>
       </c>
       <c r="K53" s="4">
-        <f>H53*J53</f>
+        <f t="shared" si="4"/>
         <v>11.7</v>
       </c>
     </row>
@@ -2352,7 +4456,7 @@
         <v>0</v>
       </c>
       <c r="K54" s="4">
-        <f>H54*J54</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2382,7 +4486,7 @@
         <v>8</v>
       </c>
       <c r="K55" s="4">
-        <f>H55*J55</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
     </row>
@@ -2409,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="4">
-        <f>H56*J56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2492,7 +4596,7 @@
         <v>0</v>
       </c>
       <c r="K61" s="4">
-        <f t="shared" ref="K61" si="3">H61*J61</f>
+        <f t="shared" ref="K61" si="5">H61*J61</f>
         <v>0</v>
       </c>
     </row>
@@ -2568,169 +4672,103 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="68" spans="1:13">
-      <c r="A68" s="5" t="s">
+    <row r="68" spans="1:13" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="14.25" customHeight="1">
+      <c r="C69" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="14.25" customHeight="1">
+      <c r="C70" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
-      <c r="B69" s="5" t="s">
+    <row r="72" spans="1:13">
+      <c r="B72" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G69" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H69" s="4">
+      <c r="G72" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H72" s="4">
         <v>19.95</v>
       </c>
-      <c r="I69" s="5">
-        <v>1</v>
-      </c>
-      <c r="J69" s="5">
+      <c r="I72" s="5">
+        <v>1</v>
+      </c>
+      <c r="J72" s="5">
         <v>4</v>
       </c>
-      <c r="K69" s="4">
-        <f>H69*J69</f>
+      <c r="K72" s="4">
+        <f>H72*J72</f>
         <v>79.8</v>
       </c>
-      <c r="M69" s="5" t="s">
+      <c r="M72" s="5" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="16.5" customHeight="1">
-      <c r="B70" s="5" t="s">
+    <row r="73" spans="1:13" ht="16.5" customHeight="1">
+      <c r="B73" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C73" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D73" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G70" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H70" s="4">
+      <c r="G73" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H73" s="4">
         <v>29.95</v>
       </c>
-      <c r="I70" s="5">
-        <v>2</v>
-      </c>
-      <c r="J70" s="5">
-        <v>0</v>
-      </c>
-      <c r="K70" s="4">
-        <f>H70*J70</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="A72" s="5" t="s">
+      <c r="I73" s="5">
+        <v>2</v>
+      </c>
+      <c r="J73" s="5">
+        <v>0</v>
+      </c>
+      <c r="K73" s="4">
+        <f>H73*J73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="5" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
-      <c r="B73" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H73" s="4">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="I73" s="5">
-        <v>100</v>
-      </c>
-      <c r="J73" s="5">
-        <v>0</v>
-      </c>
-      <c r="K73" s="4">
-        <f t="shared" ref="K73:K88" si="4">H73*J73</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="B74" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H74" s="4">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="I74" s="5">
-        <v>100</v>
-      </c>
-      <c r="J74" s="5">
-        <v>0</v>
-      </c>
-      <c r="K74" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="B75" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H75" s="4">
-        <v>8.9499999999999993</v>
-      </c>
-      <c r="I75" s="5">
-        <v>50</v>
-      </c>
-      <c r="J75" s="5">
-        <v>0</v>
-      </c>
-      <c r="K75" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:13">
       <c r="B76" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>131</v>
+        <v>16</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H76" s="4">
-        <v>2.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="I76" s="5">
         <v>100</v>
@@ -2739,19 +4777,19 @@
         <v>0</v>
       </c>
       <c r="K76" s="4">
-        <f>H76*J76</f>
+        <f t="shared" ref="K76:K91" si="6">H76*J76</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:13">
       <c r="B77" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>132</v>
+        <v>19</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>133</v>
+        <v>20</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>22</v>
@@ -2766,55 +4804,55 @@
         <v>0</v>
       </c>
       <c r="K77" s="4">
-        <f>H77*J77</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="17.25" customHeight="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
       <c r="B78" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>135</v>
+        <v>26</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H78" s="4">
-        <v>9.9499999999999993</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="I78" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J78" s="5">
         <v>0</v>
       </c>
       <c r="K78" s="4">
-        <f>H78*J78</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:13">
       <c r="B79" s="5" t="s">
-        <v>190</v>
+        <v>23</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H79" s="4">
-        <v>8.9499999999999993</v>
+        <v>2.95</v>
       </c>
       <c r="I79" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J79" s="5">
         <v>0</v>
@@ -2824,349 +4862,430 @@
         <v>0</v>
       </c>
     </row>
+    <row r="80" spans="1:13">
+      <c r="B80" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H80" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I80" s="5">
+        <v>100</v>
+      </c>
+      <c r="J80" s="5">
+        <v>0</v>
+      </c>
+      <c r="K80" s="4">
+        <f>H80*J80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="17.25" customHeight="1">
+      <c r="B81" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H81" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I81" s="5">
+        <v>100</v>
+      </c>
+      <c r="J81" s="5">
+        <v>0</v>
+      </c>
+      <c r="K81" s="4">
+        <f>H81*J81</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="82" spans="1:12">
-      <c r="A82" s="5" t="s">
+      <c r="B82" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H82" s="4">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I82" s="5">
+        <v>50</v>
+      </c>
+      <c r="J82" s="5">
+        <v>0</v>
+      </c>
+      <c r="K82" s="4">
+        <f>H82*J82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
-      <c r="B83" s="5" t="s">
+    <row r="86" spans="1:12">
+      <c r="B86" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D86" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E86" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="G83" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H83" s="4">
+      <c r="G86" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H86" s="4">
         <v>49.95</v>
       </c>
-      <c r="I83" s="5">
-        <v>1</v>
-      </c>
-      <c r="J83" s="5">
-        <v>1</v>
-      </c>
-      <c r="K83" s="4">
-        <f>H83*J83</f>
+      <c r="I86" s="5">
+        <v>1</v>
+      </c>
+      <c r="J86" s="5">
+        <v>1</v>
+      </c>
+      <c r="K86" s="4">
+        <f>H86*J86</f>
         <v>49.95</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
-      <c r="B84" s="5" t="s">
+    <row r="87" spans="1:12">
+      <c r="B87" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D87" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G84" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H84" s="4">
+      <c r="G87" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H87" s="4">
         <v>5.95</v>
       </c>
-      <c r="I84" s="5">
-        <v>1</v>
-      </c>
-      <c r="J84" s="5">
-        <v>2</v>
-      </c>
-      <c r="K84" s="4">
-        <f>H84*J84</f>
+      <c r="I87" s="5">
+        <v>1</v>
+      </c>
+      <c r="J87" s="5">
+        <v>2</v>
+      </c>
+      <c r="K87" s="4">
+        <f>H87*J87</f>
         <v>11.9</v>
       </c>
-      <c r="L84" s="11"/>
-    </row>
-    <row r="85" spans="1:12">
-      <c r="B85" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H85" s="4">
-        <v>24.95</v>
-      </c>
-      <c r="I85" s="5">
-        <v>1</v>
-      </c>
-      <c r="J85" s="5">
-        <v>1</v>
-      </c>
-      <c r="K85" s="4">
-        <f>H85*J85</f>
-        <v>24.95</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12">
-      <c r="A87" s="5" t="s">
-        <v>238</v>
-      </c>
+      <c r="L87" s="11"/>
     </row>
     <row r="88" spans="1:12">
       <c r="B88" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H88" s="4">
+        <v>24.95</v>
+      </c>
+      <c r="I88" s="5">
+        <v>1</v>
+      </c>
+      <c r="J88" s="5">
+        <v>1</v>
+      </c>
+      <c r="K88" s="4">
+        <f>H88*J88</f>
+        <v>24.95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="B91" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D91" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E91" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G88" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H88" s="4">
+      <c r="G91" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H91" s="4">
         <v>0.95</v>
       </c>
-      <c r="I88" s="5" t="s">
+      <c r="I91" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J88" s="5">
+      <c r="J91" s="5">
         <v>16</v>
       </c>
-      <c r="K88" s="4">
-        <f t="shared" si="4"/>
+      <c r="K91" s="4">
+        <f t="shared" si="6"/>
         <v>15.2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12">
-      <c r="B89" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H89" s="4">
-        <v>16.95</v>
-      </c>
-      <c r="I89" s="5">
-        <v>1</v>
-      </c>
-      <c r="J89" s="5">
-        <v>0</v>
-      </c>
-      <c r="K89" s="4">
-        <f>H89*J89</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12">
-      <c r="A91" s="5" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="92" spans="1:12">
       <c r="B92" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E92" s="5">
-        <v>346</v>
+        <v>52</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="H92" s="4">
-        <v>27.17</v>
-      </c>
-      <c r="I92" s="5" t="s">
-        <v>65</v>
+        <v>16.95</v>
+      </c>
+      <c r="I92" s="5">
+        <v>1</v>
       </c>
       <c r="J92" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K92" s="4">
         <f>H92*J92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="B95" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E95" s="5">
+        <v>346</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H95" s="4">
         <v>27.17</v>
       </c>
-    </row>
-    <row r="93" spans="1:12">
-      <c r="B93" s="5" t="s">
+      <c r="I95" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J95" s="5">
+        <v>1</v>
+      </c>
+      <c r="K95" s="4">
+        <f>H95*J95</f>
+        <v>27.17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="B96" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D93" s="6" t="s">
+      <c r="D96" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E93" s="5">
+      <c r="E96" s="5">
         <v>693</v>
       </c>
-      <c r="G93" s="5" t="s">
+      <c r="G96" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H93" s="4">
+      <c r="H96" s="4">
         <v>12.77</v>
       </c>
-      <c r="I93" s="5" t="s">
+      <c r="I96" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J93" s="5">
-        <v>0</v>
-      </c>
-      <c r="K93" s="4">
-        <f>H93*J93</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12">
-      <c r="B94" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G94" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H94" s="4">
-        <v>1.52</v>
-      </c>
-      <c r="I94" s="5">
-        <v>1</v>
-      </c>
-      <c r="J94" s="5">
-        <v>8</v>
-      </c>
-      <c r="K94" s="4">
-        <f>H94*J94</f>
-        <v>12.16</v>
+      <c r="J96" s="5">
+        <v>0</v>
+      </c>
+      <c r="K96" s="4">
+        <f>H96*J96</f>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="2:11">
       <c r="B97" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>141</v>
+        <v>70</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="H97" s="4">
-        <v>3.95</v>
+        <v>1.52</v>
       </c>
       <c r="I97" s="5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J97" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K97" s="4">
         <f>H97*J97</f>
-        <v>3.95</v>
-      </c>
-    </row>
-    <row r="98" spans="2:11">
-      <c r="B98" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H98" s="4">
-        <v>4.95</v>
-      </c>
-      <c r="I98" s="5">
-        <v>12</v>
-      </c>
-      <c r="J98" s="5">
-        <v>1</v>
-      </c>
-      <c r="K98" s="4">
-        <f>H98*J98</f>
-        <v>4.95</v>
-      </c>
-    </row>
-    <row r="99" spans="2:11">
-      <c r="B99" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G99" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H99" s="4">
-        <v>13.95</v>
-      </c>
-      <c r="I99" s="5">
-        <v>12</v>
-      </c>
-      <c r="J99" s="5">
-        <v>0</v>
-      </c>
-      <c r="K99" s="4">
-        <f>H99*J99</f>
-        <v>0</v>
+        <v>12.16</v>
       </c>
     </row>
     <row r="100" spans="2:11">
       <c r="B100" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>145</v>
+        <v>188</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>140</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H100" s="4">
-        <v>12</v>
+        <v>3.95</v>
       </c>
       <c r="I100" s="5">
         <v>12</v>
       </c>
       <c r="J100" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K100" s="4">
         <f>H100*J100</f>
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11">
+      <c r="B101" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H101" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="I101" s="5">
+        <v>12</v>
+      </c>
+      <c r="J101" s="5">
+        <v>1</v>
+      </c>
+      <c r="K101" s="4">
+        <f>H101*J101</f>
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11">
+      <c r="B102" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H102" s="4">
+        <v>13.95</v>
+      </c>
+      <c r="I102" s="5">
+        <v>12</v>
+      </c>
+      <c r="J102" s="5">
+        <v>0</v>
+      </c>
+      <c r="K102" s="4">
+        <f>H102*J102</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="2:11">
+      <c r="B103" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H103" s="4">
+        <v>12</v>
+      </c>
+      <c r="I103" s="5">
+        <v>12</v>
+      </c>
+      <c r="J103" s="5">
+        <v>0</v>
+      </c>
       <c r="K103" s="4">
-        <f>SUM(K2:K102)</f>
+        <f>H103*J103</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:11">
+      <c r="K106" s="4">
+        <f>SUM(K2:K105)</f>
         <v>1113.4800000000005</v>
       </c>
     </row>
@@ -3181,7 +5300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N85"/>
   <sheetViews>
@@ -5367,7 +7486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N79"/>
   <sheetViews>

</xml_diff>